<commit_message>
#667 On Demand Next Gen Template
</commit_message>
<xml_diff>
--- a/Logic Maps/On Demand Next Gen Work List Template.xlsx
+++ b/Logic Maps/On Demand Next Gen Work List Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAXIS-scripts\Logic Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7AAE0BDC-73BA-4ECD-A8BF-968F587173AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0625F2-E7A6-44CB-BFD5-927230C81FD6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{242310C6-257C-4D87-B2B9-A5B71458F366}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{242310C6-257C-4D87-B2B9-A5B71458F366}"/>
   </bookViews>
   <sheets>
     <sheet name="Work List for 12-8-21" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>Work List created Date</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Action Taken</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Resolve Questionable Interview</t>
   </si>
   <si>
@@ -152,6 +149,12 @@
   </si>
   <si>
     <t>CASE NUMBER</t>
+  </si>
+  <si>
+    <t>Notes on Today's Work</t>
+  </si>
+  <si>
+    <t>Cases with a Cnote added</t>
   </si>
 </sst>
 </file>
@@ -300,6 +303,411 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="m\/d\/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -325,411 +733,6 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="m\/d\/yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -750,37 +753,39 @@
     <sheetNames>
       <sheetName val="Sheet1"/>
       <sheetName val="Controls"/>
+      <sheetName val="Working Excel"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D6C2CE68-3A6A-4030-B83A-FF7200378A0E}" name="Table1" displayName="Table1" ref="A1:R7" totalsRowShown="0" headerRowDxfId="3" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D6C2CE68-3A6A-4030-B83A-FF7200378A0E}" name="Table1" displayName="Table1" ref="A1:R7" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:R7" xr:uid="{60D5FF1A-C2B8-4995-B215-9D81A0B75208}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{C47609A7-3F8E-491D-9537-17C58BF29ACE}" name="Case Worker" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{826AAF06-4EC2-484C-B2CA-A70F12C0A7F6}" name="Case Number" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{4C3C419E-9DD1-4486-9736-78983D66A63C}" name="Case Name" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{10F5763A-35A0-47FC-A5A6-AF9913FEEEC8}" name="SNAP Status" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{642B5D80-DEDC-443C-A0AF-ADBDA7FF1ADD}" name="Cash Status" dataDxfId="15"/>
-    <tableColumn id="16" xr3:uid="{225CC7C9-8C70-4670-9E8C-CFDA903E2C8B}" name="REPT PND2 Days" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{E0343797-1C6E-463D-8634-E7BB57F23202}" name="Application Date" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{A40D9281-B39B-4A3D-A85C-02E0B360D0F4}" name="Interview Date" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{C779BCF5-A6E0-4565-B507-5FAD2EA8265A}" name="Questionable Interview" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{C4D692F3-0F9C-4513-81BA-9BDFA9D9DF5B}" name="Resolve Questionable Interview" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{378615B0-B662-42B8-858A-0BC6BE347B3F}" name="Appt Notice Date" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{5CBBAEE7-F3C5-432A-9DAA-657F99EED528}" name="Date of Appt" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{8A79684B-5F3B-439A-8D39-ECB0ABD61E16}" name="NOMI Date" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{22762C73-811B-4C73-93FE-FB6746875DD2}" name="Day 30" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{C47609A7-3F8E-491D-9537-17C58BF29ACE}" name="Case Worker" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{826AAF06-4EC2-484C-B2CA-A70F12C0A7F6}" name="Case Number" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{4C3C419E-9DD1-4486-9736-78983D66A63C}" name="Case Name" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{10F5763A-35A0-47FC-A5A6-AF9913FEEEC8}" name="SNAP Status" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{642B5D80-DEDC-443C-A0AF-ADBDA7FF1ADD}" name="Cash Status" dataDxfId="13"/>
+    <tableColumn id="16" xr3:uid="{225CC7C9-8C70-4670-9E8C-CFDA903E2C8B}" name="REPT PND2 Days" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{E0343797-1C6E-463D-8634-E7BB57F23202}" name="Application Date" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{A40D9281-B39B-4A3D-A85C-02E0B360D0F4}" name="Interview Date" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{C779BCF5-A6E0-4565-B507-5FAD2EA8265A}" name="Questionable Interview" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{C4D692F3-0F9C-4513-81BA-9BDFA9D9DF5B}" name="Resolve Questionable Interview" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{378615B0-B662-42B8-858A-0BC6BE347B3F}" name="Appt Notice Date" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{5CBBAEE7-F3C5-432A-9DAA-657F99EED528}" name="Date of Appt" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{8A79684B-5F3B-439A-8D39-ECB0ABD61E16}" name="NOMI Date" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{22762C73-811B-4C73-93FE-FB6746875DD2}" name="Day 30" dataDxfId="4">
       <calculatedColumnFormula>[1]!Table2[[#This Row],[Application Date]]+30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{8E3FCA59-2961-450C-B809-183295284A01}" name="Action Taken" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{24389B76-0D5F-4479-864B-2AF7272DBDD3}" name="Notes" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{8E3FCA59-2961-450C-B809-183295284A01}" name="Action Taken" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{24389B76-0D5F-4479-864B-2AF7272DBDD3}" name="Notes on Today's Work" dataDxfId="2"/>
     <tableColumn id="17" xr3:uid="{70BCBF6D-1D6A-4946-98A4-1F8EBE2A0808}" name="Email correction sent to" dataDxfId="1"/>
     <tableColumn id="18" xr3:uid="{505B9D9C-D67D-4AE0-A71F-4C8665896DC0}" name="Email Correction Regarding" dataDxfId="0"/>
   </tableColumns>
@@ -1087,8 +1092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8070B74E-64DC-4F54-9A48-587FFB51CB42}">
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1130,7 +1135,7 @@
         <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>7</v>
@@ -1142,7 +1147,7 @@
         <v>9</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>10</v>
@@ -1160,24 +1165,24 @@
         <v>16</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="Q1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R1" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>13</v>
@@ -1212,13 +1217,13 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>14</v>
@@ -1251,13 +1256,13 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="C4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>14</v>
@@ -1290,13 +1295,13 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="C5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
@@ -1329,13 +1334,13 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="C6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>13</v>
@@ -1370,13 +1375,13 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="C7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
@@ -1417,10 +1422,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3C6355-F678-4C3D-8F25-996512EC9851}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1447,7 +1452,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>150</v>
@@ -1455,7 +1460,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>25</v>
@@ -1463,7 +1468,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -1471,7 +1476,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>50</v>
@@ -1479,7 +1484,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7">
         <v>50</v>
@@ -1487,7 +1492,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8">
         <v>20</v>
@@ -1495,12 +1500,12 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="8">
         <v>0.52083333333333337</v>
@@ -1508,27 +1513,32 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>